<commit_message>
convert the code to functions
</commit_message>
<xml_diff>
--- a/tournament/points_table.xlsx
+++ b/tournament/points_table.xlsx
@@ -474,7 +474,7 @@
         <v>11</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -489,7 +489,7 @@
         <v>15</v>
       </c>
       <c r="H2">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -506,7 +506,7 @@
         <v>12</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -521,7 +521,7 @@
         <v>16</v>
       </c>
       <c r="H3">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -538,7 +538,7 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -553,7 +553,7 @@
         <v>17</v>
       </c>
       <c r="H4">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -570,7 +570,7 @@
         <v>14</v>
       </c>
       <c r="B5">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -585,7 +585,7 @@
         <v>18</v>
       </c>
       <c r="H5">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I5">
         <v>0</v>

</xml_diff>